<commit_message>
adding new cdtede command to broadcast stop data taking to canisters
</commit_message>
<xml_diff>
--- a/commands/cdtede/cdtede_command_deck.xlsx
+++ b/commands/cdtede/cdtede_command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi-4matter/foxsi4-commands/commands/cdtede/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD2C387-6772-AF4D-9946-4BE1B78B3498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2F67EE-093D-4047-B62E-9064F66AF111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17900" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="109">
   <si>
     <t>R=1/W=0</t>
   </si>
@@ -352,6 +352,15 @@
   </si>
   <si>
     <t>0x20</t>
+  </si>
+  <si>
+    <t>set_can_broadcast_readout_stop</t>
+  </si>
+  <si>
+    <t>0x3c3c0101050505053c3c3c3c</t>
+  </si>
+  <si>
+    <t>ALL canisters stop reading out.</t>
   </si>
 </sst>
 </file>
@@ -824,13 +833,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283F008E-2DBD-E446-BC2F-AA0D9FF4122A}">
-  <dimension ref="A1:AC23"/>
+  <dimension ref="A1:AC24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AC7" sqref="AC7"/>
+      <selection pane="bottomRight" activeCell="AC17" sqref="AC17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1476,7 +1485,7 @@
         <v>1000</v>
       </c>
       <c r="E9" s="3" t="str">
-        <f t="shared" ref="E9:E23" si="1">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C9,7) + BIN2DEC($D9)))</f>
+        <f t="shared" ref="E9:E24" si="1">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C9,7) + BIN2DEC($D9)))</f>
         <v>0x8</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -2184,7 +2193,7 @@
     </row>
     <row r="17" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>48</v>
+        <v>106</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>33</v>
@@ -2193,11 +2202,11 @@
         <v>0</v>
       </c>
       <c r="D17" s="10">
-        <v>10011</v>
+        <v>10111</v>
       </c>
       <c r="E17" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x13</v>
+        <v>0x17</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>15</v>
@@ -2263,18 +2272,18 @@
         <v>53</v>
       </c>
       <c r="AA17" s="23" t="s">
-        <v>70</v>
+        <v>107</v>
       </c>
       <c r="AB17" t="s">
         <v>35</v>
       </c>
       <c r="AC17" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>33</v>
@@ -2283,11 +2292,11 @@
         <v>0</v>
       </c>
       <c r="D18" s="10">
-        <v>10100</v>
+        <v>10011</v>
       </c>
       <c r="E18" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x14</v>
+        <v>0x13</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>15</v>
@@ -2353,18 +2362,18 @@
         <v>53</v>
       </c>
       <c r="AA18" s="23" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="AB18" t="s">
         <v>35</v>
       </c>
       <c r="AC18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>33</v>
@@ -2373,11 +2382,11 @@
         <v>0</v>
       </c>
       <c r="D19" s="10">
-        <v>10101</v>
+        <v>10100</v>
       </c>
       <c r="E19" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x15</v>
+        <v>0x14</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>15</v>
@@ -2443,18 +2452,18 @@
         <v>53</v>
       </c>
       <c r="AA19" s="23" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="AB19" t="s">
         <v>35</v>
       </c>
       <c r="AC19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="26" t="s">
-        <v>51</v>
+      <c r="A20" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>33</v>
@@ -2463,11 +2472,11 @@
         <v>0</v>
       </c>
       <c r="D20" s="10">
-        <v>10110</v>
+        <v>10101</v>
       </c>
       <c r="E20" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x16</v>
+        <v>0x15</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>15</v>
@@ -2533,18 +2542,18 @@
         <v>53</v>
       </c>
       <c r="AA20" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AB20" t="s">
         <v>35</v>
       </c>
       <c r="AC20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="26" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>33</v>
@@ -2555,8 +2564,9 @@
       <c r="D21" s="10">
         <v>10110</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>94</v>
+      <c r="E21" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0x16</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>15</v>
@@ -2622,18 +2632,18 @@
         <v>53</v>
       </c>
       <c r="AA21" s="23" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="AB21" t="s">
         <v>35</v>
       </c>
       <c r="AC21" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>33</v>
@@ -2645,7 +2655,7 @@
         <v>10110</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>15</v>
@@ -2711,18 +2721,18 @@
         <v>53</v>
       </c>
       <c r="AA22" s="23" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AB22" t="s">
         <v>35</v>
       </c>
       <c r="AC22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>52</v>
+      <c r="A23" s="26" t="s">
+        <v>93</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>33</v>
@@ -2731,82 +2741,171 @@
         <v>0</v>
       </c>
       <c r="D23" s="10">
+        <v>10110</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="L23" s="6">
+        <v>0</v>
+      </c>
+      <c r="M23" s="6">
+        <v>0</v>
+      </c>
+      <c r="N23" s="6">
+        <v>0</v>
+      </c>
+      <c r="O23" s="6">
+        <v>0</v>
+      </c>
+      <c r="P23" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="6">
+        <v>0</v>
+      </c>
+      <c r="R23" s="6">
+        <v>0</v>
+      </c>
+      <c r="S23" s="6">
+        <v>0</v>
+      </c>
+      <c r="T23" s="6">
+        <v>1</v>
+      </c>
+      <c r="U23" s="6">
+        <v>0</v>
+      </c>
+      <c r="V23" s="6">
+        <v>0</v>
+      </c>
+      <c r="W23" s="16">
+        <v>0</v>
+      </c>
+      <c r="X23" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y23" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z23" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA23" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0</v>
+      </c>
+      <c r="D24" s="10">
         <v>100001</v>
       </c>
-      <c r="E23" s="3" t="str">
+      <c r="E24" s="3" t="str">
         <f t="shared" si="1"/>
         <v>0x21</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G23" t="s">
-        <v>15</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K23" s="23" t="s">
+      <c r="F24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K24" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="L23" s="6">
-        <v>0</v>
-      </c>
-      <c r="M23" s="6">
-        <v>0</v>
-      </c>
-      <c r="N23" s="6">
-        <v>0</v>
-      </c>
-      <c r="O23" s="6">
-        <v>0</v>
-      </c>
-      <c r="P23" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="6">
-        <v>0</v>
-      </c>
-      <c r="R23" s="6">
-        <v>0</v>
-      </c>
-      <c r="S23" s="6">
-        <v>0</v>
-      </c>
-      <c r="T23" s="6">
+      <c r="L24" s="6">
+        <v>0</v>
+      </c>
+      <c r="M24" s="6">
+        <v>0</v>
+      </c>
+      <c r="N24" s="6">
+        <v>0</v>
+      </c>
+      <c r="O24" s="6">
+        <v>0</v>
+      </c>
+      <c r="P24" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="6">
+        <v>0</v>
+      </c>
+      <c r="R24" s="6">
+        <v>0</v>
+      </c>
+      <c r="S24" s="6">
+        <v>0</v>
+      </c>
+      <c r="T24" s="6">
         <v>1</v>
       </c>
-      <c r="U23" s="6">
-        <v>0</v>
-      </c>
-      <c r="V23" s="6">
-        <v>0</v>
-      </c>
-      <c r="W23" s="16">
-        <v>0</v>
-      </c>
-      <c r="X23" s="13" t="s">
+      <c r="U24" s="6">
+        <v>0</v>
+      </c>
+      <c r="V24" s="6">
+        <v>0</v>
+      </c>
+      <c r="W24" s="16">
+        <v>0</v>
+      </c>
+      <c r="X24" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="Y23" s="3" t="s">
+      <c r="Y24" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="Z23" s="3" t="s">
+      <c r="Z24" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AA23" s="23" t="s">
+      <c r="AA24" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AB23" t="s">
+      <c r="AB24" t="s">
         <v>35</v>
       </c>
-      <c r="AC23" t="s">
+      <c r="AC24" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
patch v1.1.0 with smaller max_payload_bytes
- smaller max_payload_bytes values are now also consistent between
ethernet_interface definitions and spacewire_interface definitions, so
FramePacketizer creates downlink packets correctly.

- housekeeping data ping packet definitions are retained.
</commit_message>
<xml_diff>
--- a/commands/cdtede/cdtede_command_deck.xlsx
+++ b/commands/cdtede/cdtede_command_deck.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/GSE/GSE-FOXSI-4/foxsi4-commands/commands/cdtede/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi-4matter/foxsi4-commands/commands/cdtede/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968B0234-F90C-4C42-993E-E1675CC32BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A006B95-51B7-F347-82AA-0CD166B24A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17900" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17880" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
   <sheets>
     <sheet name="all_systems" sheetId="1" r:id="rId1"/>
@@ -1088,7 +1088,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1143,14 +1143,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1468,10 +1460,10 @@
   <dimension ref="A1:AE116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="T3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AC3" sqref="AC3"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L1:W1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1493,8 +1485,8 @@
     <col min="25" max="25" width="12.83203125" style="20" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="11.1640625" style="20" customWidth="1"/>
     <col min="27" max="27" width="27.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.5" style="35" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.1640625" style="35" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.5" style="20" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.1640625" style="20" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="19.1640625" customWidth="1"/>
     <col min="31" max="31" width="73.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1537,8 +1529,8 @@
       </c>
       <c r="Z1" s="28"/>
       <c r="AA1" s="29"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
     </row>
     <row r="2" spans="1:31" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1622,10 +1614,10 @@
       <c r="AA2" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="AB2" s="31" t="s">
+      <c r="AB2" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="AC2" s="31" t="s">
+      <c r="AC2" s="1" t="s">
         <v>314</v>
       </c>
       <c r="AD2" s="1" t="s">
@@ -1718,10 +1710,10 @@
       <c r="AA3" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="AB3" s="32">
+      <c r="AB3" s="26">
         <v>22</v>
       </c>
-      <c r="AC3" s="32" t="s">
+      <c r="AC3" s="26" t="s">
         <v>316</v>
       </c>
       <c r="AD3" t="s">
@@ -1814,10 +1806,10 @@
       <c r="AA4" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="AB4" s="32">
+      <c r="AB4" s="26">
         <v>23</v>
       </c>
-      <c r="AC4" s="32" t="s">
+      <c r="AC4" s="26" t="s">
         <v>316</v>
       </c>
       <c r="AD4" t="s">
@@ -1910,10 +1902,10 @@
       <c r="AA5" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="AB5" s="32">
+      <c r="AB5" s="26">
         <v>24</v>
       </c>
-      <c r="AC5" s="32" t="s">
+      <c r="AC5" s="26" t="s">
         <v>316</v>
       </c>
       <c r="AD5" t="s">
@@ -2006,10 +1998,10 @@
       <c r="AA6" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="AB6" s="32">
+      <c r="AB6" s="26">
         <v>25</v>
       </c>
-      <c r="AC6" s="32" t="s">
+      <c r="AC6" s="26" t="s">
         <v>316</v>
       </c>
       <c r="AD6" t="s">
@@ -2102,10 +2094,10 @@
       <c r="AA7" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="AB7" s="32">
+      <c r="AB7" s="26">
         <v>26</v>
       </c>
-      <c r="AC7" s="32" t="s">
+      <c r="AC7" s="26" t="s">
         <v>316</v>
       </c>
       <c r="AD7" t="s">
@@ -2198,10 +2190,10 @@
       <c r="AA8" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="AB8" s="32">
+      <c r="AB8" s="26">
         <v>27</v>
       </c>
-      <c r="AC8" s="32" t="s">
+      <c r="AC8" s="26" t="s">
         <v>316</v>
       </c>
       <c r="AD8" t="s">
@@ -2238,8 +2230,8 @@
       <c r="Y9" s="24"/>
       <c r="Z9" s="7"/>
       <c r="AA9" s="24"/>
-      <c r="AB9" s="33"/>
-      <c r="AC9" s="33"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="7"/>
     </row>
     <row r="10" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
@@ -2324,7 +2316,7 @@
       <c r="AA10" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="AB10" s="34">
+      <c r="AB10" s="3">
         <v>16</v>
       </c>
       <c r="AC10" s="26" t="s">
@@ -2420,7 +2412,7 @@
       <c r="AA11" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="AB11" s="34">
+      <c r="AB11" s="3">
         <v>1</v>
       </c>
       <c r="AC11" s="26" t="s">
@@ -2516,7 +2508,7 @@
       <c r="AA12" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="AB12" s="34">
+      <c r="AB12" s="3">
         <v>2</v>
       </c>
       <c r="AC12" s="26" t="s">
@@ -2612,7 +2604,7 @@
       <c r="AA13" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="AB13" s="34">
+      <c r="AB13" s="3">
         <v>7</v>
       </c>
       <c r="AC13" s="26" t="s">
@@ -2708,7 +2700,7 @@
       <c r="AA14" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="AB14" s="34">
+      <c r="AB14" s="3">
         <v>14</v>
       </c>
       <c r="AC14" s="26" t="s">
@@ -2804,7 +2796,7 @@
       <c r="AA15" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="AB15" s="34">
+      <c r="AB15" s="3">
         <v>15</v>
       </c>
       <c r="AC15" s="26" t="s">
@@ -2900,7 +2892,7 @@
       <c r="AA16" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="AB16" s="34">
+      <c r="AB16" s="3">
         <v>10</v>
       </c>
       <c r="AC16" s="26" t="s">
@@ -2996,7 +2988,7 @@
       <c r="AA17" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="AB17" s="34">
+      <c r="AB17" s="3">
         <v>11</v>
       </c>
       <c r="AC17" s="26" t="s">
@@ -3092,7 +3084,7 @@
       <c r="AA18" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="AB18" s="34">
+      <c r="AB18" s="3">
         <v>12</v>
       </c>
       <c r="AC18" s="26" t="s">
@@ -3188,7 +3180,7 @@
       <c r="AA19" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="AB19" s="34">
+      <c r="AB19" s="3">
         <v>13</v>
       </c>
       <c r="AC19" s="26" t="s">
@@ -3284,7 +3276,7 @@
       <c r="AA20" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="AB20" s="34">
+      <c r="AB20" s="3">
         <v>3</v>
       </c>
       <c r="AC20" s="26" t="s">
@@ -3380,7 +3372,7 @@
       <c r="AA21" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="AB21" s="34">
+      <c r="AB21" s="3">
         <v>4</v>
       </c>
       <c r="AC21" s="26" t="s">
@@ -3476,7 +3468,7 @@
       <c r="AA22" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="AB22" s="34">
+      <c r="AB22" s="3">
         <v>5</v>
       </c>
       <c r="AC22" s="26" t="s">
@@ -3572,7 +3564,7 @@
       <c r="AA23" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="AB23" s="34">
+      <c r="AB23" s="3">
         <v>6</v>
       </c>
       <c r="AC23" s="26" t="s">
@@ -3668,7 +3660,7 @@
       <c r="AA24" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="AB24" s="34">
+      <c r="AB24" s="3">
         <v>8</v>
       </c>
       <c r="AC24" s="26" t="s">
@@ -3764,7 +3756,7 @@
       <c r="AA25" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="AB25" s="34">
+      <c r="AB25" s="3">
         <v>9</v>
       </c>
       <c r="AC25" s="26" t="s">
@@ -3860,7 +3852,7 @@
       <c r="AA26" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="AB26" s="34">
+      <c r="AB26" s="3">
         <v>31</v>
       </c>
       <c r="AC26" s="26" t="s">
@@ -3956,7 +3948,7 @@
       <c r="AA27" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="AB27" s="34">
+      <c r="AB27" s="3">
         <v>32</v>
       </c>
       <c r="AC27" s="26" t="s">
@@ -4052,7 +4044,7 @@
       <c r="AA28" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="AB28" s="34">
+      <c r="AB28" s="3">
         <v>33</v>
       </c>
       <c r="AC28" s="26" t="s">
@@ -4148,7 +4140,7 @@
       <c r="AA29" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="AB29" s="34">
+      <c r="AB29" s="3">
         <v>34</v>
       </c>
       <c r="AC29" s="26" t="s">
@@ -4244,7 +4236,7 @@
       <c r="AA30" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="AB30" s="34">
+      <c r="AB30" s="3">
         <v>35</v>
       </c>
       <c r="AC30" s="26" t="s">
@@ -4340,7 +4332,7 @@
       <c r="AA31" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="AB31" s="34">
+      <c r="AB31" s="3">
         <v>36</v>
       </c>
       <c r="AC31" s="26" t="s">
@@ -4436,7 +4428,7 @@
       <c r="AA32" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="AB32" s="34">
+      <c r="AB32" s="3">
         <v>37</v>
       </c>
       <c r="AC32" s="26" t="s">
@@ -4532,7 +4524,7 @@
       <c r="AA33" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="AB33" s="34">
+      <c r="AB33" s="3">
         <v>38</v>
       </c>
       <c r="AC33" s="26" t="s">
@@ -4628,7 +4620,7 @@
       <c r="AA34" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="AB34" s="34">
+      <c r="AB34" s="3">
         <v>39</v>
       </c>
       <c r="AC34" s="26" t="s">
@@ -4724,7 +4716,7 @@
       <c r="AA35" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="AB35" s="34">
+      <c r="AB35" s="3">
         <v>40</v>
       </c>
       <c r="AC35" s="26" t="s">
@@ -4820,7 +4812,7 @@
       <c r="AA36" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="AB36" s="34">
+      <c r="AB36" s="3">
         <v>41</v>
       </c>
       <c r="AC36" s="26" t="s">
@@ -4916,7 +4908,7 @@
       <c r="AA37" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="AB37" s="34">
+      <c r="AB37" s="3">
         <v>42</v>
       </c>
       <c r="AC37" s="26" t="s">
@@ -5012,7 +5004,7 @@
       <c r="AA38" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="AB38" s="34">
+      <c r="AB38" s="3">
         <v>43</v>
       </c>
       <c r="AC38" s="26" t="s">
@@ -5108,7 +5100,7 @@
       <c r="AA39" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="AB39" s="34">
+      <c r="AB39" s="3">
         <v>44</v>
       </c>
       <c r="AC39" s="26" t="s">
@@ -5204,7 +5196,7 @@
       <c r="AA40" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="AB40" s="34">
+      <c r="AB40" s="3">
         <v>45</v>
       </c>
       <c r="AC40" s="26" t="s">
@@ -5300,7 +5292,7 @@
       <c r="AA41" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="AB41" s="34">
+      <c r="AB41" s="3">
         <v>46</v>
       </c>
       <c r="AC41" s="26" t="s">
@@ -5396,7 +5388,7 @@
       <c r="AA42" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="AB42" s="34">
+      <c r="AB42" s="3">
         <v>17</v>
       </c>
       <c r="AC42" s="26" t="s">
@@ -5492,7 +5484,7 @@
       <c r="AA43" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="AB43" s="34">
+      <c r="AB43" s="3">
         <v>28</v>
       </c>
       <c r="AC43" s="26" t="s">
@@ -5588,7 +5580,7 @@
       <c r="AA44" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="AB44" s="34">
+      <c r="AB44" s="3">
         <v>29</v>
       </c>
       <c r="AC44" s="26" t="s">
@@ -5684,7 +5676,7 @@
       <c r="AA45" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="AB45" s="34">
+      <c r="AB45" s="3">
         <v>30</v>
       </c>
       <c r="AC45" s="26" t="s">
@@ -5780,7 +5772,7 @@
       <c r="AA46" s="23" t="s">
         <v>172</v>
       </c>
-      <c r="AB46" s="34">
+      <c r="AB46" s="3">
         <v>18</v>
       </c>
       <c r="AC46" s="26" t="s">
@@ -5876,7 +5868,7 @@
       <c r="AA47" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="AB47" s="34">
+      <c r="AB47" s="3">
         <v>19</v>
       </c>
       <c r="AC47" s="26" t="s">
@@ -5972,7 +5964,7 @@
       <c r="AA48" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="AB48" s="34">
+      <c r="AB48" s="3">
         <v>20</v>
       </c>
       <c r="AC48" s="26" t="s">
@@ -6068,7 +6060,7 @@
       <c r="AA49" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="AB49" s="34">
+      <c r="AB49" s="3">
         <v>21</v>
       </c>
       <c r="AC49" s="26" t="s">
@@ -6164,7 +6156,7 @@
       <c r="AA50" s="23" t="s">
         <v>245</v>
       </c>
-      <c r="AB50" s="34">
+      <c r="AB50" s="3">
         <v>47</v>
       </c>
       <c r="AC50" s="26" t="s">
@@ -6256,7 +6248,7 @@
       <c r="AA51" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="AB51" s="34">
+      <c r="AB51" s="3">
         <v>48</v>
       </c>
       <c r="AC51" s="26" t="s">
@@ -6348,7 +6340,7 @@
       <c r="AA52" s="23" t="s">
         <v>247</v>
       </c>
-      <c r="AB52" s="34">
+      <c r="AB52" s="3">
         <v>49</v>
       </c>
       <c r="AC52" s="26" t="s">
@@ -6440,7 +6432,7 @@
       <c r="AA53" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="AB53" s="34">
+      <c r="AB53" s="3">
         <v>50</v>
       </c>
       <c r="AC53" s="26" t="s">
@@ -6532,7 +6524,7 @@
       <c r="AA54" s="25" t="s">
         <v>249</v>
       </c>
-      <c r="AB54" s="34">
+      <c r="AB54" s="3">
         <v>51</v>
       </c>
       <c r="AC54" s="26" t="s">
@@ -6624,7 +6616,7 @@
       <c r="AA55" s="23" t="s">
         <v>250</v>
       </c>
-      <c r="AB55" s="34">
+      <c r="AB55" s="3">
         <v>52</v>
       </c>
       <c r="AC55" s="26" t="s">
@@ -6716,7 +6708,7 @@
       <c r="AA56" s="23" t="s">
         <v>251</v>
       </c>
-      <c r="AB56" s="34">
+      <c r="AB56" s="3">
         <v>53</v>
       </c>
       <c r="AC56" s="26" t="s">
@@ -6808,7 +6800,7 @@
       <c r="AA57" s="23" t="s">
         <v>252</v>
       </c>
-      <c r="AB57" s="34">
+      <c r="AB57" s="3">
         <v>54</v>
       </c>
       <c r="AC57" s="26" t="s">
@@ -6900,7 +6892,7 @@
       <c r="AA58" s="23" t="s">
         <v>253</v>
       </c>
-      <c r="AB58" s="34">
+      <c r="AB58" s="3">
         <v>55</v>
       </c>
       <c r="AC58" s="26" t="s">
@@ -6992,7 +6984,7 @@
       <c r="AA59" s="25" t="s">
         <v>254</v>
       </c>
-      <c r="AB59" s="34">
+      <c r="AB59" s="3">
         <v>56</v>
       </c>
       <c r="AC59" s="26" t="s">
@@ -7084,7 +7076,7 @@
       <c r="AA60" s="23" t="s">
         <v>255</v>
       </c>
-      <c r="AB60" s="34">
+      <c r="AB60" s="3">
         <v>57</v>
       </c>
       <c r="AC60" s="26" t="s">
@@ -7176,7 +7168,7 @@
       <c r="AA61" s="23" t="s">
         <v>256</v>
       </c>
-      <c r="AB61" s="34">
+      <c r="AB61" s="3">
         <v>58</v>
       </c>
       <c r="AC61" s="26" t="s">
@@ -7268,7 +7260,7 @@
       <c r="AA62" s="23" t="s">
         <v>257</v>
       </c>
-      <c r="AB62" s="34">
+      <c r="AB62" s="3">
         <v>59</v>
       </c>
       <c r="AC62" s="26" t="s">
@@ -7360,7 +7352,7 @@
       <c r="AA63" s="23" t="s">
         <v>258</v>
       </c>
-      <c r="AB63" s="34">
+      <c r="AB63" s="3">
         <v>60</v>
       </c>
       <c r="AC63" s="26" t="s">
@@ -7452,7 +7444,7 @@
       <c r="AA64" s="25" t="s">
         <v>259</v>
       </c>
-      <c r="AB64" s="34">
+      <c r="AB64" s="3">
         <v>61</v>
       </c>
       <c r="AC64" s="26" t="s">
@@ -7544,7 +7536,7 @@
       <c r="AA65" s="25" t="s">
         <v>260</v>
       </c>
-      <c r="AB65" s="34">
+      <c r="AB65" s="3">
         <v>62</v>
       </c>
       <c r="AC65" s="26" t="s">
@@ -7636,7 +7628,7 @@
       <c r="AA66" s="25" t="s">
         <v>261</v>
       </c>
-      <c r="AB66" s="34">
+      <c r="AB66" s="3">
         <v>63</v>
       </c>
       <c r="AC66" s="26" t="s">
@@ -7728,7 +7720,7 @@
       <c r="AA67" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="AB67" s="34">
+      <c r="AB67" s="3">
         <v>64</v>
       </c>
       <c r="AC67" s="26" t="s">
@@ -7820,7 +7812,7 @@
       <c r="AA68" s="25" t="s">
         <v>263</v>
       </c>
-      <c r="AB68" s="34">
+      <c r="AB68" s="3">
         <v>65</v>
       </c>
       <c r="AC68" s="26" t="s">
@@ -7912,7 +7904,7 @@
       <c r="AA69" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="AB69" s="34">
+      <c r="AB69" s="3">
         <v>66</v>
       </c>
       <c r="AC69" s="26" t="s">
@@ -8004,7 +7996,7 @@
       <c r="AA70" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="AB70" s="34">
+      <c r="AB70" s="3">
         <v>67</v>
       </c>
       <c r="AC70" s="26" t="s">
@@ -8096,7 +8088,7 @@
       <c r="AA71" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="AB71" s="34">
+      <c r="AB71" s="3">
         <v>68</v>
       </c>
       <c r="AC71" s="26" t="s">
@@ -8188,7 +8180,7 @@
       <c r="AA72" s="25" t="s">
         <v>267</v>
       </c>
-      <c r="AB72" s="34">
+      <c r="AB72" s="3">
         <v>69</v>
       </c>
       <c r="AC72" s="26" t="s">
@@ -8280,7 +8272,7 @@
       <c r="AA73" s="25" t="s">
         <v>268</v>
       </c>
-      <c r="AB73" s="34">
+      <c r="AB73" s="3">
         <v>70</v>
       </c>
       <c r="AC73" s="26" t="s">
@@ -8372,7 +8364,7 @@
       <c r="AA74" s="25" t="s">
         <v>269</v>
       </c>
-      <c r="AB74" s="34">
+      <c r="AB74" s="3">
         <v>71</v>
       </c>
       <c r="AC74" s="26" t="s">
@@ -8464,7 +8456,7 @@
       <c r="AA75" s="25" t="s">
         <v>273</v>
       </c>
-      <c r="AB75" s="34">
+      <c r="AB75" s="3">
         <v>72</v>
       </c>
       <c r="AC75" s="26" t="s">
@@ -8556,7 +8548,7 @@
       <c r="AA76" s="25" t="s">
         <v>274</v>
       </c>
-      <c r="AB76" s="34">
+      <c r="AB76" s="3">
         <v>73</v>
       </c>
       <c r="AC76" s="26" t="s">
@@ -8648,7 +8640,7 @@
       <c r="AA77" s="25" t="s">
         <v>275</v>
       </c>
-      <c r="AB77" s="34">
+      <c r="AB77" s="3">
         <v>74</v>
       </c>
       <c r="AC77" s="26" t="s">
@@ -8740,7 +8732,7 @@
       <c r="AA78" s="25" t="s">
         <v>276</v>
       </c>
-      <c r="AB78" s="34">
+      <c r="AB78" s="3">
         <v>75</v>
       </c>
       <c r="AC78" s="26" t="s">
@@ -8832,7 +8824,7 @@
       <c r="AA79" s="25" t="s">
         <v>277</v>
       </c>
-      <c r="AB79" s="34">
+      <c r="AB79" s="3">
         <v>76</v>
       </c>
       <c r="AC79" s="26" t="s">
@@ -8924,7 +8916,7 @@
       <c r="AA80" s="25" t="s">
         <v>278</v>
       </c>
-      <c r="AB80" s="34">
+      <c r="AB80" s="3">
         <v>77</v>
       </c>
       <c r="AC80" s="26" t="s">
@@ -9016,7 +9008,7 @@
       <c r="AA81" s="25" t="s">
         <v>279</v>
       </c>
-      <c r="AB81" s="34">
+      <c r="AB81" s="3">
         <v>78</v>
       </c>
       <c r="AC81" s="26" t="s">
@@ -9108,7 +9100,7 @@
       <c r="AA82" s="25" t="s">
         <v>280</v>
       </c>
-      <c r="AB82" s="34">
+      <c r="AB82" s="3">
         <v>79</v>
       </c>
       <c r="AC82" s="26" t="s">
@@ -9200,7 +9192,7 @@
       <c r="AA83" s="25" t="s">
         <v>281</v>
       </c>
-      <c r="AB83" s="34">
+      <c r="AB83" s="3">
         <v>80</v>
       </c>
       <c r="AC83" s="26" t="s">
@@ -9292,7 +9284,7 @@
       <c r="AA84" s="25" t="s">
         <v>282</v>
       </c>
-      <c r="AB84" s="34">
+      <c r="AB84" s="3">
         <v>81</v>
       </c>
       <c r="AC84" s="26" t="s">
@@ -9384,7 +9376,7 @@
       <c r="AA85" s="25" t="s">
         <v>283</v>
       </c>
-      <c r="AB85" s="34">
+      <c r="AB85" s="3">
         <v>82</v>
       </c>
       <c r="AC85" s="26" t="s">
@@ -9476,7 +9468,7 @@
       <c r="AA86" s="25" t="s">
         <v>284</v>
       </c>
-      <c r="AB86" s="34">
+      <c r="AB86" s="3">
         <v>83</v>
       </c>
       <c r="AC86" s="26" t="s">
@@ -9568,7 +9560,7 @@
       <c r="AA87" s="25" t="s">
         <v>285</v>
       </c>
-      <c r="AB87" s="34">
+      <c r="AB87" s="3">
         <v>84</v>
       </c>
       <c r="AC87" s="26" t="s">
@@ -9660,7 +9652,7 @@
       <c r="AA88" s="25" t="s">
         <v>286</v>
       </c>
-      <c r="AB88" s="34">
+      <c r="AB88" s="3">
         <v>85</v>
       </c>
       <c r="AC88" s="26" t="s">
@@ -9752,7 +9744,7 @@
       <c r="AA89" s="25" t="s">
         <v>287</v>
       </c>
-      <c r="AB89" s="34">
+      <c r="AB89" s="3">
         <v>86</v>
       </c>
       <c r="AC89" s="26" t="s">
@@ -9844,7 +9836,7 @@
       <c r="AA90" s="25" t="s">
         <v>288</v>
       </c>
-      <c r="AB90" s="34">
+      <c r="AB90" s="3">
         <v>87</v>
       </c>
       <c r="AC90" s="26" t="s">
@@ -9936,7 +9928,7 @@
       <c r="AA91" s="25" t="s">
         <v>289</v>
       </c>
-      <c r="AB91" s="34">
+      <c r="AB91" s="3">
         <v>88</v>
       </c>
       <c r="AC91" s="26" t="s">
@@ -10028,7 +10020,7 @@
       <c r="AA92" s="25" t="s">
         <v>290</v>
       </c>
-      <c r="AB92" s="34">
+      <c r="AB92" s="3">
         <v>89</v>
       </c>
       <c r="AC92" s="26" t="s">
@@ -10120,7 +10112,7 @@
       <c r="AA93" s="25" t="s">
         <v>291</v>
       </c>
-      <c r="AB93" s="34">
+      <c r="AB93" s="3">
         <v>90</v>
       </c>
       <c r="AC93" s="26" t="s">
@@ -10212,7 +10204,7 @@
       <c r="AA94" s="25" t="s">
         <v>292</v>
       </c>
-      <c r="AB94" s="34">
+      <c r="AB94" s="3">
         <v>91</v>
       </c>
       <c r="AC94" s="26" t="s">
@@ -10304,7 +10296,7 @@
       <c r="AA95" s="25" t="s">
         <v>293</v>
       </c>
-      <c r="AB95" s="34">
+      <c r="AB95" s="3">
         <v>92</v>
       </c>
       <c r="AC95" s="26" t="s">
@@ -10396,7 +10388,7 @@
       <c r="AA96" s="25" t="s">
         <v>294</v>
       </c>
-      <c r="AB96" s="34">
+      <c r="AB96" s="3">
         <v>93</v>
       </c>
       <c r="AC96" s="26" t="s">
@@ -10488,7 +10480,7 @@
       <c r="AA97" s="25" t="s">
         <v>295</v>
       </c>
-      <c r="AB97" s="34">
+      <c r="AB97" s="3">
         <v>94</v>
       </c>
       <c r="AC97" s="26" t="s">
@@ -10580,7 +10572,7 @@
       <c r="AA98" s="25" t="s">
         <v>296</v>
       </c>
-      <c r="AB98" s="34">
+      <c r="AB98" s="3">
         <v>95</v>
       </c>
       <c r="AC98" s="26" t="s">
@@ -10672,7 +10664,7 @@
       <c r="AA99" s="25" t="s">
         <v>297</v>
       </c>
-      <c r="AB99" s="34">
+      <c r="AB99" s="3">
         <v>96</v>
       </c>
       <c r="AC99" s="26" t="s">
@@ -10764,7 +10756,7 @@
       <c r="AA100" s="25" t="s">
         <v>298</v>
       </c>
-      <c r="AB100" s="34">
+      <c r="AB100" s="3">
         <v>97</v>
       </c>
       <c r="AC100" s="26" t="s">
@@ -10856,7 +10848,7 @@
       <c r="AA101" s="25" t="s">
         <v>299</v>
       </c>
-      <c r="AB101" s="34">
+      <c r="AB101" s="3">
         <v>98</v>
       </c>
       <c r="AC101" s="26" t="s">
@@ -10948,7 +10940,7 @@
       <c r="AA102" s="25" t="s">
         <v>300</v>
       </c>
-      <c r="AB102" s="34">
+      <c r="AB102" s="3">
         <v>99</v>
       </c>
       <c r="AC102" s="26" t="s">
@@ -11040,7 +11032,7 @@
       <c r="AA103" s="25" t="s">
         <v>301</v>
       </c>
-      <c r="AB103" s="34">
+      <c r="AB103" s="3">
         <v>100</v>
       </c>
       <c r="AC103" s="26" t="s">
@@ -11132,7 +11124,7 @@
       <c r="AA104" s="25" t="s">
         <v>302</v>
       </c>
-      <c r="AB104" s="34">
+      <c r="AB104" s="3">
         <v>101</v>
       </c>
       <c r="AC104" s="26" t="s">
@@ -11224,7 +11216,7 @@
       <c r="AA105" s="25" t="s">
         <v>303</v>
       </c>
-      <c r="AB105" s="34">
+      <c r="AB105" s="3">
         <v>102</v>
       </c>
       <c r="AC105" s="26" t="s">
@@ -11316,7 +11308,7 @@
       <c r="AA106" s="25" t="s">
         <v>304</v>
       </c>
-      <c r="AB106" s="34">
+      <c r="AB106" s="3">
         <v>103</v>
       </c>
       <c r="AC106" s="26" t="s">
@@ -11408,7 +11400,7 @@
       <c r="AA107" s="25" t="s">
         <v>305</v>
       </c>
-      <c r="AB107" s="34">
+      <c r="AB107" s="3">
         <v>104</v>
       </c>
       <c r="AC107" s="26" t="s">
@@ -11500,7 +11492,7 @@
       <c r="AA108" s="25" t="s">
         <v>306</v>
       </c>
-      <c r="AB108" s="34">
+      <c r="AB108" s="3">
         <v>105</v>
       </c>
       <c r="AC108" s="26" t="s">
@@ -11592,7 +11584,7 @@
       <c r="AA109" s="25" t="s">
         <v>307</v>
       </c>
-      <c r="AB109" s="34">
+      <c r="AB109" s="3">
         <v>106</v>
       </c>
       <c r="AC109" s="26" t="s">
@@ -11684,7 +11676,7 @@
       <c r="AA110" s="25" t="s">
         <v>308</v>
       </c>
-      <c r="AB110" s="34">
+      <c r="AB110" s="3">
         <v>107</v>
       </c>
       <c r="AC110" s="26" t="s">
@@ -11776,7 +11768,7 @@
       <c r="AA111" s="25" t="s">
         <v>309</v>
       </c>
-      <c r="AB111" s="34">
+      <c r="AB111" s="3">
         <v>108</v>
       </c>
       <c r="AC111" s="26" t="s">
@@ -11868,7 +11860,7 @@
       <c r="AA112" s="25" t="s">
         <v>310</v>
       </c>
-      <c r="AB112" s="34">
+      <c r="AB112" s="3">
         <v>109</v>
       </c>
       <c r="AC112" s="26" t="s">
@@ -11960,7 +11952,7 @@
       <c r="AA113" s="25" t="s">
         <v>311</v>
       </c>
-      <c r="AB113" s="34">
+      <c r="AB113" s="3">
         <v>110</v>
       </c>
       <c r="AC113" s="26" t="s">
@@ -12052,7 +12044,7 @@
       <c r="AA114" s="25" t="s">
         <v>312</v>
       </c>
-      <c r="AB114" s="34">
+      <c r="AB114" s="3">
         <v>111</v>
       </c>
       <c r="AC114" s="26" t="s">
@@ -12144,7 +12136,7 @@
       <c r="AA115" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="AB115" s="34">
+      <c r="AB115" s="3">
         <v>112</v>
       </c>
       <c r="AC115" s="26" t="s">

</xml_diff>

<commit_message>
adding CdTe DE broadcast reset pointer command. Validator now checks for order to be strictly monotone
</commit_message>
<xml_diff>
--- a/commands/cdtede/cdtede_command_deck.xlsx
+++ b/commands/cdtede/cdtede_command_deck.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi-4matter/foxsi4-commands/commands/cdtede/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A006B95-51B7-F347-82AA-0CD166B24A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40782A6C-FE5F-DD4A-93D9-949F7D81BA18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17880" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1587" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1602" uniqueCount="320">
   <si>
     <t>R=1/W=0</t>
   </si>
@@ -985,6 +985,15 @@
   </si>
   <si>
     <t>0x000000</t>
+  </si>
+  <si>
+    <t>ALL canisters reset pointer regardless of observation status</t>
+  </si>
+  <si>
+    <t>0x3c3c01000c0c0c0c3c3c3c3c</t>
+  </si>
+  <si>
+    <t>set_can_broadcast_rst_ptr</t>
   </si>
 </sst>
 </file>
@@ -1457,13 +1466,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283F008E-2DBD-E446-BC2F-AA0D9FF4122A}">
-  <dimension ref="A1:AE116"/>
+  <dimension ref="A1:AE117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="S42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L2" sqref="L1:W1048576"/>
+      <selection pane="bottomRight" activeCell="AD74" sqref="AD74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1711,7 +1720,7 @@
         <v>21</v>
       </c>
       <c r="AB3" s="26">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AC3" s="26" t="s">
         <v>316</v>
@@ -1807,7 +1816,7 @@
         <v>21</v>
       </c>
       <c r="AB4" s="26">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AC4" s="26" t="s">
         <v>316</v>
@@ -1903,7 +1912,7 @@
         <v>21</v>
       </c>
       <c r="AB5" s="26">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AC5" s="26" t="s">
         <v>316</v>
@@ -1999,7 +2008,7 @@
         <v>21</v>
       </c>
       <c r="AB6" s="26">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AC6" s="26" t="s">
         <v>316</v>
@@ -2095,7 +2104,7 @@
         <v>21</v>
       </c>
       <c r="AB7" s="26">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC7" s="26" t="s">
         <v>316</v>
@@ -2191,7 +2200,7 @@
         <v>21</v>
       </c>
       <c r="AB8" s="26">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AC8" s="26" t="s">
         <v>316</v>
@@ -2247,7 +2256,7 @@
         <v>1000</v>
       </c>
       <c r="E10" s="3" t="str">
-        <f t="shared" ref="E10:E115" si="1">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C10,7) + BIN2DEC($D10)))</f>
+        <f t="shared" ref="E10:E116" si="1">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C10,7) + BIN2DEC($D10)))</f>
         <v>0x8</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -2317,7 +2326,7 @@
         <v>54</v>
       </c>
       <c r="AB10" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AC10" s="26" t="s">
         <v>316</v>
@@ -2701,7 +2710,7 @@
         <v>58</v>
       </c>
       <c r="AB14" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AC14" s="26" t="s">
         <v>316</v>
@@ -2797,7 +2806,7 @@
         <v>59</v>
       </c>
       <c r="AB15" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AC15" s="26" t="s">
         <v>316</v>
@@ -3003,7 +3012,7 @@
     </row>
     <row r="18" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>47</v>
+        <v>319</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>33</v>
@@ -3012,11 +3021,11 @@
         <v>0</v>
       </c>
       <c r="D18" s="10">
-        <v>10010</v>
+        <v>11011</v>
       </c>
       <c r="E18" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x12</v>
+        <v>0x1B</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>15</v>
@@ -3082,7 +3091,7 @@
         <v>53</v>
       </c>
       <c r="AA18" s="23" t="s">
-        <v>69</v>
+        <v>318</v>
       </c>
       <c r="AB18" s="3">
         <v>12</v>
@@ -3094,12 +3103,12 @@
         <v>35</v>
       </c>
       <c r="AE18" t="s">
-        <v>68</v>
+        <v>317</v>
       </c>
     </row>
     <row r="19" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>104</v>
+        <v>47</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>33</v>
@@ -3108,11 +3117,11 @@
         <v>0</v>
       </c>
       <c r="D19" s="10">
-        <v>10111</v>
+        <v>10010</v>
       </c>
       <c r="E19" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x17</v>
+        <v>0x12</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>15</v>
@@ -3178,7 +3187,7 @@
         <v>53</v>
       </c>
       <c r="AA19" s="23" t="s">
-        <v>105</v>
+        <v>69</v>
       </c>
       <c r="AB19" s="3">
         <v>13</v>
@@ -3190,12 +3199,12 @@
         <v>35</v>
       </c>
       <c r="AE19" t="s">
-        <v>106</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>48</v>
+        <v>104</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>33</v>
@@ -3204,11 +3213,11 @@
         <v>0</v>
       </c>
       <c r="D20" s="10">
-        <v>10011</v>
+        <v>10111</v>
       </c>
       <c r="E20" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x13</v>
+        <v>0x17</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>15</v>
@@ -3274,10 +3283,10 @@
         <v>53</v>
       </c>
       <c r="AA20" s="23" t="s">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="AB20" s="3">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="AC20" s="26" t="s">
         <v>316</v>
@@ -3286,12 +3295,12 @@
         <v>35</v>
       </c>
       <c r="AE20" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>33</v>
@@ -3300,11 +3309,11 @@
         <v>0</v>
       </c>
       <c r="D21" s="10">
-        <v>10100</v>
+        <v>10011</v>
       </c>
       <c r="E21" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x14</v>
+        <v>0x13</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>15</v>
@@ -3370,10 +3379,10 @@
         <v>53</v>
       </c>
       <c r="AA21" s="23" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="AB21" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC21" s="26" t="s">
         <v>316</v>
@@ -3382,12 +3391,12 @@
         <v>35</v>
       </c>
       <c r="AE21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>33</v>
@@ -3396,11 +3405,11 @@
         <v>0</v>
       </c>
       <c r="D22" s="10">
-        <v>10101</v>
+        <v>10100</v>
       </c>
       <c r="E22" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x15</v>
+        <v>0x14</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>15</v>
@@ -3466,24 +3475,24 @@
         <v>53</v>
       </c>
       <c r="AA22" s="23" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="AB22" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AC22" s="26" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="AD22" t="s">
         <v>35</v>
       </c>
       <c r="AE22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:31" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="26" t="s">
-        <v>51</v>
+      <c r="A23" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>33</v>
@@ -3492,11 +3501,11 @@
         <v>0</v>
       </c>
       <c r="D23" s="10">
-        <v>10110</v>
+        <v>10101</v>
       </c>
       <c r="E23" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x16</v>
+        <v>0x15</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>15</v>
@@ -3562,10 +3571,10 @@
         <v>53</v>
       </c>
       <c r="AA23" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AB23" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AC23" s="26" t="s">
         <v>315</v>
@@ -3574,12 +3583,12 @@
         <v>35</v>
       </c>
       <c r="AE23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="26" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>33</v>
@@ -3588,11 +3597,11 @@
         <v>0</v>
       </c>
       <c r="D24" s="10">
-        <v>11000</v>
+        <v>10110</v>
       </c>
       <c r="E24" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x18</v>
+        <v>0x16</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>15</v>
@@ -3658,24 +3667,24 @@
         <v>53</v>
       </c>
       <c r="AA24" s="23" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="AB24" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AC24" s="26" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AD24" t="s">
         <v>35</v>
       </c>
       <c r="AE24" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>33</v>
@@ -3684,11 +3693,11 @@
         <v>0</v>
       </c>
       <c r="D25" s="10">
-        <v>11001</v>
+        <v>11000</v>
       </c>
       <c r="E25" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x19</v>
+        <v>0x18</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>15</v>
@@ -3754,10 +3763,10 @@
         <v>53</v>
       </c>
       <c r="AA25" s="23" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AB25" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AC25" s="26" t="s">
         <v>316</v>
@@ -3766,12 +3775,12 @@
         <v>35</v>
       </c>
       <c r="AE25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="26" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>33</v>
@@ -3780,11 +3789,11 @@
         <v>0</v>
       </c>
       <c r="D26" s="10">
-        <v>100000</v>
+        <v>11001</v>
       </c>
       <c r="E26" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x20</v>
+        <v>0x19</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>15</v>
@@ -3850,10 +3859,10 @@
         <v>53</v>
       </c>
       <c r="AA26" s="23" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="AB26" s="3">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="AC26" s="26" t="s">
         <v>316</v>
@@ -3861,13 +3870,13 @@
       <c r="AD26" t="s">
         <v>35</v>
       </c>
-      <c r="AE26" s="3" t="s">
-        <v>125</v>
+      <c r="AE26" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B27" s="18" t="s">
         <v>33</v>
@@ -3876,11 +3885,11 @@
         <v>0</v>
       </c>
       <c r="D27" s="10">
-        <v>100001</v>
+        <v>100000</v>
       </c>
       <c r="E27" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x21</v>
+        <v>0x20</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>15</v>
@@ -3946,7 +3955,7 @@
         <v>53</v>
       </c>
       <c r="AA27" s="23" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="AB27" s="3">
         <v>32</v>
@@ -3958,12 +3967,12 @@
         <v>35</v>
       </c>
       <c r="AE27" s="3" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B28" s="18" t="s">
         <v>33</v>
@@ -3972,11 +3981,11 @@
         <v>0</v>
       </c>
       <c r="D28" s="10">
-        <v>100010</v>
+        <v>100001</v>
       </c>
       <c r="E28" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x22</v>
+        <v>0x21</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>15</v>
@@ -4042,7 +4051,7 @@
         <v>53</v>
       </c>
       <c r="AA28" s="23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AB28" s="3">
         <v>33</v>
@@ -4054,12 +4063,12 @@
         <v>35</v>
       </c>
       <c r="AE28" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B29" s="18" t="s">
         <v>33</v>
@@ -4068,11 +4077,11 @@
         <v>0</v>
       </c>
       <c r="D29" s="10">
-        <v>100011</v>
+        <v>100010</v>
       </c>
       <c r="E29" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x23</v>
+        <v>0x22</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>15</v>
@@ -4138,7 +4147,7 @@
         <v>53</v>
       </c>
       <c r="AA29" s="23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AB29" s="3">
         <v>34</v>
@@ -4150,12 +4159,12 @@
         <v>35</v>
       </c>
       <c r="AE29" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B30" s="18" t="s">
         <v>33</v>
@@ -4164,11 +4173,11 @@
         <v>0</v>
       </c>
       <c r="D30" s="10">
-        <v>100100</v>
+        <v>100011</v>
       </c>
       <c r="E30" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x24</v>
+        <v>0x23</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>15</v>
@@ -4234,7 +4243,7 @@
         <v>53</v>
       </c>
       <c r="AA30" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AB30" s="3">
         <v>35</v>
@@ -4246,12 +4255,12 @@
         <v>35</v>
       </c>
       <c r="AE30" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B31" s="18" t="s">
         <v>33</v>
@@ -4260,11 +4269,11 @@
         <v>0</v>
       </c>
       <c r="D31" s="10">
-        <v>100101</v>
+        <v>100100</v>
       </c>
       <c r="E31" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x25</v>
+        <v>0x24</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>15</v>
@@ -4330,7 +4339,7 @@
         <v>53</v>
       </c>
       <c r="AA31" s="23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AB31" s="3">
         <v>36</v>
@@ -4342,12 +4351,12 @@
         <v>35</v>
       </c>
       <c r="AE31" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B32" s="18" t="s">
         <v>33</v>
@@ -4356,11 +4365,11 @@
         <v>0</v>
       </c>
       <c r="D32" s="10">
-        <v>100110</v>
+        <v>100101</v>
       </c>
       <c r="E32" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x26</v>
+        <v>0x25</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>15</v>
@@ -4426,7 +4435,7 @@
         <v>53</v>
       </c>
       <c r="AA32" s="23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AB32" s="3">
         <v>37</v>
@@ -4438,12 +4447,12 @@
         <v>35</v>
       </c>
       <c r="AE32" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B33" s="18" t="s">
         <v>33</v>
@@ -4452,11 +4461,11 @@
         <v>0</v>
       </c>
       <c r="D33" s="10">
-        <v>100111</v>
+        <v>100110</v>
       </c>
       <c r="E33" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x27</v>
+        <v>0x26</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>15</v>
@@ -4522,7 +4531,7 @@
         <v>53</v>
       </c>
       <c r="AA33" s="23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AB33" s="3">
         <v>38</v>
@@ -4534,12 +4543,12 @@
         <v>35</v>
       </c>
       <c r="AE33" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B34" s="18" t="s">
         <v>33</v>
@@ -4548,11 +4557,11 @@
         <v>0</v>
       </c>
       <c r="D34" s="10">
-        <v>101000</v>
+        <v>100111</v>
       </c>
       <c r="E34" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x28</v>
+        <v>0x27</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>15</v>
@@ -4618,7 +4627,7 @@
         <v>53</v>
       </c>
       <c r="AA34" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AB34" s="3">
         <v>39</v>
@@ -4630,12 +4639,12 @@
         <v>35</v>
       </c>
       <c r="AE34" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B35" s="18" t="s">
         <v>33</v>
@@ -4644,11 +4653,11 @@
         <v>0</v>
       </c>
       <c r="D35" s="10">
-        <v>101001</v>
+        <v>101000</v>
       </c>
       <c r="E35" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x29</v>
+        <v>0x28</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>15</v>
@@ -4714,7 +4723,7 @@
         <v>53</v>
       </c>
       <c r="AA35" s="23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AB35" s="3">
         <v>40</v>
@@ -4726,12 +4735,12 @@
         <v>35</v>
       </c>
       <c r="AE35" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="36" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B36" s="18" t="s">
         <v>33</v>
@@ -4740,11 +4749,11 @@
         <v>0</v>
       </c>
       <c r="D36" s="10">
-        <v>101010</v>
+        <v>101001</v>
       </c>
       <c r="E36" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x2A</v>
+        <v>0x29</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>15</v>
@@ -4810,7 +4819,7 @@
         <v>53</v>
       </c>
       <c r="AA36" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AB36" s="3">
         <v>41</v>
@@ -4822,12 +4831,12 @@
         <v>35</v>
       </c>
       <c r="AE36" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="37" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B37" s="18" t="s">
         <v>33</v>
@@ -4836,11 +4845,11 @@
         <v>0</v>
       </c>
       <c r="D37" s="10">
-        <v>101011</v>
+        <v>101010</v>
       </c>
       <c r="E37" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x2B</v>
+        <v>0x2A</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>15</v>
@@ -4906,7 +4915,7 @@
         <v>53</v>
       </c>
       <c r="AA37" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AB37" s="3">
         <v>42</v>
@@ -4918,12 +4927,12 @@
         <v>35</v>
       </c>
       <c r="AE37" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B38" s="18" t="s">
         <v>33</v>
@@ -4932,11 +4941,11 @@
         <v>0</v>
       </c>
       <c r="D38" s="10">
-        <v>101100</v>
+        <v>101011</v>
       </c>
       <c r="E38" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x2C</v>
+        <v>0x2B</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>15</v>
@@ -5002,7 +5011,7 @@
         <v>53</v>
       </c>
       <c r="AA38" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AB38" s="3">
         <v>43</v>
@@ -5014,12 +5023,12 @@
         <v>35</v>
       </c>
       <c r="AE38" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="39" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B39" s="18" t="s">
         <v>33</v>
@@ -5028,11 +5037,11 @@
         <v>0</v>
       </c>
       <c r="D39" s="10">
-        <v>101101</v>
+        <v>101100</v>
       </c>
       <c r="E39" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x2D</v>
+        <v>0x2C</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>15</v>
@@ -5098,7 +5107,7 @@
         <v>53</v>
       </c>
       <c r="AA39" s="23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AB39" s="3">
         <v>44</v>
@@ -5110,12 +5119,12 @@
         <v>35</v>
       </c>
       <c r="AE39" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="40" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B40" s="18" t="s">
         <v>33</v>
@@ -5124,11 +5133,11 @@
         <v>0</v>
       </c>
       <c r="D40" s="10">
-        <v>101110</v>
+        <v>101101</v>
       </c>
       <c r="E40" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x2E</v>
+        <v>0x2D</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>15</v>
@@ -5194,7 +5203,7 @@
         <v>53</v>
       </c>
       <c r="AA40" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AB40" s="3">
         <v>45</v>
@@ -5206,12 +5215,12 @@
         <v>35</v>
       </c>
       <c r="AE40" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B41" s="18" t="s">
         <v>33</v>
@@ -5220,11 +5229,11 @@
         <v>0</v>
       </c>
       <c r="D41" s="10">
-        <v>101111</v>
+        <v>101110</v>
       </c>
       <c r="E41" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x2F</v>
+        <v>0x2E</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>15</v>
@@ -5290,7 +5299,7 @@
         <v>53</v>
       </c>
       <c r="AA41" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AB41" s="3">
         <v>46</v>
@@ -5302,12 +5311,12 @@
         <v>35</v>
       </c>
       <c r="AE41" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="42" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B42" s="18" t="s">
         <v>33</v>
@@ -5316,11 +5325,11 @@
         <v>0</v>
       </c>
       <c r="D42" s="10">
-        <v>110000</v>
+        <v>101111</v>
       </c>
       <c r="E42" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x30</v>
+        <v>0x2F</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>15</v>
@@ -5386,10 +5395,10 @@
         <v>53</v>
       </c>
       <c r="AA42" s="23" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="AB42" s="3">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="AC42" s="26" t="s">
         <v>316</v>
@@ -5398,12 +5407,12 @@
         <v>35</v>
       </c>
       <c r="AE42" s="3" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="43" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="26" t="s">
-        <v>156</v>
+        <v>123</v>
       </c>
       <c r="B43" s="18" t="s">
         <v>33</v>
@@ -5412,11 +5421,11 @@
         <v>0</v>
       </c>
       <c r="D43" s="10">
-        <v>110001</v>
+        <v>110000</v>
       </c>
       <c r="E43" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x31</v>
+        <v>0x30</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>15</v>
@@ -5482,10 +5491,10 @@
         <v>53</v>
       </c>
       <c r="AA43" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AB43" s="3">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="AC43" s="26" t="s">
         <v>316</v>
@@ -5494,12 +5503,12 @@
         <v>35</v>
       </c>
       <c r="AE43" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B44" s="18" t="s">
         <v>33</v>
@@ -5508,11 +5517,11 @@
         <v>0</v>
       </c>
       <c r="D44" s="10">
-        <v>110010</v>
+        <v>110001</v>
       </c>
       <c r="E44" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x32</v>
+        <v>0x31</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>15</v>
@@ -5578,7 +5587,7 @@
         <v>53</v>
       </c>
       <c r="AA44" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AB44" s="3">
         <v>29</v>
@@ -5595,7 +5604,7 @@
     </row>
     <row r="45" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B45" s="18" t="s">
         <v>33</v>
@@ -5604,11 +5613,11 @@
         <v>0</v>
       </c>
       <c r="D45" s="10">
-        <v>110100</v>
+        <v>110010</v>
       </c>
       <c r="E45" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x34</v>
+        <v>0x32</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>15</v>
@@ -5674,7 +5683,7 @@
         <v>53</v>
       </c>
       <c r="AA45" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AB45" s="3">
         <v>30</v>
@@ -5691,7 +5700,7 @@
     </row>
     <row r="46" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="26" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B46" s="18" t="s">
         <v>33</v>
@@ -5700,11 +5709,11 @@
         <v>0</v>
       </c>
       <c r="D46" s="10">
-        <v>11</v>
+        <v>110100</v>
       </c>
       <c r="E46" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x3</v>
+        <v>0x34</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>15</v>
@@ -5770,24 +5779,24 @@
         <v>53</v>
       </c>
       <c r="AA46" s="23" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="AB46" s="3">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="AC46" s="26" t="s">
         <v>316</v>
       </c>
-      <c r="AD46" s="3" t="s">
+      <c r="AD46" t="s">
         <v>35</v>
       </c>
       <c r="AE46" s="3" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="47" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="26" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B47" s="18" t="s">
         <v>33</v>
@@ -5796,11 +5805,11 @@
         <v>0</v>
       </c>
       <c r="D47" s="10">
-        <v>101</v>
+        <v>11</v>
       </c>
       <c r="E47" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x5</v>
+        <v>0x3</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>15</v>
@@ -5866,24 +5875,24 @@
         <v>53</v>
       </c>
       <c r="AA47" s="23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AB47" s="3">
         <v>19</v>
       </c>
       <c r="AC47" s="26" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="AD47" s="3" t="s">
         <v>35</v>
       </c>
       <c r="AE47" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="48" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B48" s="18" t="s">
         <v>33</v>
@@ -5892,11 +5901,11 @@
         <v>0</v>
       </c>
       <c r="D48" s="10">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E48" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x6</v>
+        <v>0x5</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>15</v>
@@ -5962,7 +5971,7 @@
         <v>53</v>
       </c>
       <c r="AA48" s="23" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="AB48" s="3">
         <v>20</v>
@@ -5974,12 +5983,12 @@
         <v>35</v>
       </c>
       <c r="AE48" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="49" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B49" s="18" t="s">
         <v>33</v>
@@ -5988,11 +5997,11 @@
         <v>0</v>
       </c>
       <c r="D49" s="10">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E49" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x7</v>
+        <v>0x6</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>15</v>
@@ -6058,7 +6067,7 @@
         <v>53</v>
       </c>
       <c r="AA49" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AB49" s="3">
         <v>21</v>
@@ -6070,12 +6079,12 @@
         <v>35</v>
       </c>
       <c r="AE49" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="50" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="26" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B50" s="18" t="s">
         <v>33</v>
@@ -6084,11 +6093,11 @@
         <v>0</v>
       </c>
       <c r="D50" s="10">
-        <v>1000000</v>
+        <v>111</v>
       </c>
       <c r="E50" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x40</v>
+        <v>0x7</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>15</v>
@@ -6154,20 +6163,24 @@
         <v>53</v>
       </c>
       <c r="AA50" s="23" t="s">
-        <v>245</v>
+        <v>179</v>
       </c>
       <c r="AB50" s="3">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="AC50" s="26" t="s">
-        <v>316</v>
-      </c>
-      <c r="AD50" s="3"/>
-      <c r="AE50" s="3"/>
+        <v>315</v>
+      </c>
+      <c r="AD50" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE50" s="3" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="51" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="26" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B51" s="18" t="s">
         <v>33</v>
@@ -6176,11 +6189,11 @@
         <v>0</v>
       </c>
       <c r="D51" s="10">
-        <v>1000001</v>
+        <v>1000000</v>
       </c>
       <c r="E51" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x41</v>
+        <v>0x40</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>15</v>
@@ -6246,7 +6259,7 @@
         <v>53</v>
       </c>
       <c r="AA51" s="23" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AB51" s="3">
         <v>48</v>
@@ -6259,7 +6272,7 @@
     </row>
     <row r="52" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="26" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B52" s="18" t="s">
         <v>33</v>
@@ -6268,11 +6281,11 @@
         <v>0</v>
       </c>
       <c r="D52" s="10">
-        <v>1000010</v>
+        <v>1000001</v>
       </c>
       <c r="E52" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x42</v>
+        <v>0x41</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>15</v>
@@ -6338,7 +6351,7 @@
         <v>53</v>
       </c>
       <c r="AA52" s="23" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AB52" s="3">
         <v>49</v>
@@ -6351,7 +6364,7 @@
     </row>
     <row r="53" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="26" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B53" s="18" t="s">
         <v>33</v>
@@ -6360,11 +6373,11 @@
         <v>0</v>
       </c>
       <c r="D53" s="10">
-        <v>1000011</v>
+        <v>1000010</v>
       </c>
       <c r="E53" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x43</v>
+        <v>0x42</v>
       </c>
       <c r="F53" s="3" t="s">
         <v>15</v>
@@ -6430,7 +6443,7 @@
         <v>53</v>
       </c>
       <c r="AA53" s="23" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AB53" s="3">
         <v>50</v>
@@ -6443,7 +6456,7 @@
     </row>
     <row r="54" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B54" s="18" t="s">
         <v>33</v>
@@ -6452,11 +6465,11 @@
         <v>0</v>
       </c>
       <c r="D54" s="10">
-        <v>1000100</v>
+        <v>1000011</v>
       </c>
       <c r="E54" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x44</v>
+        <v>0x43</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>15</v>
@@ -6521,8 +6534,8 @@
       <c r="Z54" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AA54" s="25" t="s">
-        <v>249</v>
+      <c r="AA54" s="23" t="s">
+        <v>248</v>
       </c>
       <c r="AB54" s="3">
         <v>51</v>
@@ -6535,7 +6548,7 @@
     </row>
     <row r="55" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B55" s="18" t="s">
         <v>33</v>
@@ -6544,11 +6557,11 @@
         <v>0</v>
       </c>
       <c r="D55" s="10">
-        <v>1000101</v>
+        <v>1000100</v>
       </c>
       <c r="E55" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x45</v>
+        <v>0x44</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>15</v>
@@ -6613,8 +6626,8 @@
       <c r="Z55" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AA55" s="23" t="s">
-        <v>250</v>
+      <c r="AA55" s="25" t="s">
+        <v>249</v>
       </c>
       <c r="AB55" s="3">
         <v>52</v>
@@ -6627,7 +6640,7 @@
     </row>
     <row r="56" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="26" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B56" s="18" t="s">
         <v>33</v>
@@ -6636,11 +6649,11 @@
         <v>0</v>
       </c>
       <c r="D56" s="10">
-        <v>1000110</v>
+        <v>1000101</v>
       </c>
       <c r="E56" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x46</v>
+        <v>0x45</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>15</v>
@@ -6706,7 +6719,7 @@
         <v>53</v>
       </c>
       <c r="AA56" s="23" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AB56" s="3">
         <v>53</v>
@@ -6719,7 +6732,7 @@
     </row>
     <row r="57" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="26" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B57" s="18" t="s">
         <v>33</v>
@@ -6728,11 +6741,11 @@
         <v>0</v>
       </c>
       <c r="D57" s="10">
-        <v>1000111</v>
+        <v>1000110</v>
       </c>
       <c r="E57" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x47</v>
+        <v>0x46</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>15</v>
@@ -6798,7 +6811,7 @@
         <v>53</v>
       </c>
       <c r="AA57" s="23" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AB57" s="3">
         <v>54</v>
@@ -6811,7 +6824,7 @@
     </row>
     <row r="58" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="26" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B58" s="18" t="s">
         <v>33</v>
@@ -6820,11 +6833,11 @@
         <v>0</v>
       </c>
       <c r="D58" s="10">
-        <v>1001000</v>
+        <v>1000111</v>
       </c>
       <c r="E58" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x48</v>
+        <v>0x47</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>15</v>
@@ -6890,7 +6903,7 @@
         <v>53</v>
       </c>
       <c r="AA58" s="23" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AB58" s="3">
         <v>55</v>
@@ -6903,7 +6916,7 @@
     </row>
     <row r="59" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B59" s="18" t="s">
         <v>33</v>
@@ -6912,11 +6925,11 @@
         <v>0</v>
       </c>
       <c r="D59" s="10">
-        <v>1001001</v>
+        <v>1001000</v>
       </c>
       <c r="E59" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x49</v>
+        <v>0x48</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>15</v>
@@ -6981,8 +6994,8 @@
       <c r="Z59" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AA59" s="25" t="s">
-        <v>254</v>
+      <c r="AA59" s="23" t="s">
+        <v>253</v>
       </c>
       <c r="AB59" s="3">
         <v>56</v>
@@ -6995,7 +7008,7 @@
     </row>
     <row r="60" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="26" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B60" s="18" t="s">
         <v>33</v>
@@ -7004,11 +7017,11 @@
         <v>0</v>
       </c>
       <c r="D60" s="10">
-        <v>1001010</v>
+        <v>1001001</v>
       </c>
       <c r="E60" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x4A</v>
+        <v>0x49</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>15</v>
@@ -7073,8 +7086,8 @@
       <c r="Z60" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AA60" s="23" t="s">
-        <v>255</v>
+      <c r="AA60" s="25" t="s">
+        <v>254</v>
       </c>
       <c r="AB60" s="3">
         <v>57</v>
@@ -7087,7 +7100,7 @@
     </row>
     <row r="61" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="26" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B61" s="18" t="s">
         <v>33</v>
@@ -7096,11 +7109,11 @@
         <v>0</v>
       </c>
       <c r="D61" s="10">
-        <v>1001011</v>
+        <v>1001010</v>
       </c>
       <c r="E61" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x4B</v>
+        <v>0x4A</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>15</v>
@@ -7166,7 +7179,7 @@
         <v>53</v>
       </c>
       <c r="AA61" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="AB61" s="3">
         <v>58</v>
@@ -7179,7 +7192,7 @@
     </row>
     <row r="62" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="26" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B62" s="18" t="s">
         <v>33</v>
@@ -7188,11 +7201,11 @@
         <v>0</v>
       </c>
       <c r="D62" s="10">
-        <v>1001100</v>
+        <v>1001011</v>
       </c>
       <c r="E62" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x4C</v>
+        <v>0x4B</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>15</v>
@@ -7258,7 +7271,7 @@
         <v>53</v>
       </c>
       <c r="AA62" s="23" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AB62" s="3">
         <v>59</v>
@@ -7271,7 +7284,7 @@
     </row>
     <row r="63" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="26" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="B63" s="18" t="s">
         <v>33</v>
@@ -7280,11 +7293,11 @@
         <v>0</v>
       </c>
       <c r="D63" s="10">
-        <v>1001101</v>
+        <v>1001100</v>
       </c>
       <c r="E63" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x4D</v>
+        <v>0x4C</v>
       </c>
       <c r="F63" s="3" t="s">
         <v>15</v>
@@ -7350,7 +7363,7 @@
         <v>53</v>
       </c>
       <c r="AA63" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AB63" s="3">
         <v>60</v>
@@ -7363,7 +7376,7 @@
     </row>
     <row r="64" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="26" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B64" s="18" t="s">
         <v>33</v>
@@ -7372,11 +7385,11 @@
         <v>0</v>
       </c>
       <c r="D64" s="10">
-        <v>1001110</v>
+        <v>1001101</v>
       </c>
       <c r="E64" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x4E</v>
+        <v>0x4D</v>
       </c>
       <c r="F64" s="3" t="s">
         <v>15</v>
@@ -7441,8 +7454,8 @@
       <c r="Z64" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AA64" s="25" t="s">
-        <v>259</v>
+      <c r="AA64" s="23" t="s">
+        <v>258</v>
       </c>
       <c r="AB64" s="3">
         <v>61</v>
@@ -7455,7 +7468,7 @@
     </row>
     <row r="65" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="26" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="B65" s="18" t="s">
         <v>33</v>
@@ -7464,11 +7477,11 @@
         <v>0</v>
       </c>
       <c r="D65" s="10">
-        <v>1001111</v>
+        <v>1001110</v>
       </c>
       <c r="E65" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x4F</v>
+        <v>0x4E</v>
       </c>
       <c r="F65" s="3" t="s">
         <v>15</v>
@@ -7534,7 +7547,7 @@
         <v>53</v>
       </c>
       <c r="AA65" s="25" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB65" s="3">
         <v>62</v>
@@ -7547,7 +7560,7 @@
     </row>
     <row r="66" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="26" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B66" s="18" t="s">
         <v>33</v>
@@ -7556,11 +7569,11 @@
         <v>0</v>
       </c>
       <c r="D66" s="10">
-        <v>1010000</v>
+        <v>1001111</v>
       </c>
       <c r="E66" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x50</v>
+        <v>0x4F</v>
       </c>
       <c r="F66" s="3" t="s">
         <v>15</v>
@@ -7626,7 +7639,7 @@
         <v>53</v>
       </c>
       <c r="AA66" s="25" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AB66" s="3">
         <v>63</v>
@@ -7639,7 +7652,7 @@
     </row>
     <row r="67" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="26" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B67" s="18" t="s">
         <v>33</v>
@@ -7648,11 +7661,11 @@
         <v>0</v>
       </c>
       <c r="D67" s="10">
-        <v>1010001</v>
+        <v>1010000</v>
       </c>
       <c r="E67" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x51</v>
+        <v>0x50</v>
       </c>
       <c r="F67" s="3" t="s">
         <v>15</v>
@@ -7718,7 +7731,7 @@
         <v>53</v>
       </c>
       <c r="AA67" s="25" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AB67" s="3">
         <v>64</v>
@@ -7731,7 +7744,7 @@
     </row>
     <row r="68" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="26" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B68" s="18" t="s">
         <v>33</v>
@@ -7740,11 +7753,11 @@
         <v>0</v>
       </c>
       <c r="D68" s="10">
-        <v>1010010</v>
+        <v>1010001</v>
       </c>
       <c r="E68" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x52</v>
+        <v>0x51</v>
       </c>
       <c r="F68" s="3" t="s">
         <v>15</v>
@@ -7810,7 +7823,7 @@
         <v>53</v>
       </c>
       <c r="AA68" s="25" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AB68" s="3">
         <v>65</v>
@@ -7823,7 +7836,7 @@
     </row>
     <row r="69" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="26" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="B69" s="18" t="s">
         <v>33</v>
@@ -7832,11 +7845,11 @@
         <v>0</v>
       </c>
       <c r="D69" s="10">
-        <v>1010011</v>
+        <v>1010010</v>
       </c>
       <c r="E69" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x53</v>
+        <v>0x52</v>
       </c>
       <c r="F69" s="3" t="s">
         <v>15</v>
@@ -7902,7 +7915,7 @@
         <v>53</v>
       </c>
       <c r="AA69" s="25" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AB69" s="3">
         <v>66</v>
@@ -7915,7 +7928,7 @@
     </row>
     <row r="70" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="26" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="B70" s="18" t="s">
         <v>33</v>
@@ -7924,11 +7937,11 @@
         <v>0</v>
       </c>
       <c r="D70" s="10">
-        <v>1010100</v>
+        <v>1010011</v>
       </c>
       <c r="E70" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x54</v>
+        <v>0x53</v>
       </c>
       <c r="F70" s="3" t="s">
         <v>15</v>
@@ -7994,7 +8007,7 @@
         <v>53</v>
       </c>
       <c r="AA70" s="25" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AB70" s="3">
         <v>67</v>
@@ -8007,7 +8020,7 @@
     </row>
     <row r="71" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="26" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B71" s="18" t="s">
         <v>33</v>
@@ -8016,11 +8029,11 @@
         <v>0</v>
       </c>
       <c r="D71" s="10">
-        <v>1010101</v>
+        <v>1010100</v>
       </c>
       <c r="E71" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x55</v>
+        <v>0x54</v>
       </c>
       <c r="F71" s="3" t="s">
         <v>15</v>
@@ -8086,7 +8099,7 @@
         <v>53</v>
       </c>
       <c r="AA71" s="25" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AB71" s="3">
         <v>68</v>
@@ -8099,7 +8112,7 @@
     </row>
     <row r="72" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B72" s="18" t="s">
         <v>33</v>
@@ -8108,11 +8121,11 @@
         <v>0</v>
       </c>
       <c r="D72" s="10">
-        <v>1010110</v>
+        <v>1010101</v>
       </c>
       <c r="E72" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x56</v>
+        <v>0x55</v>
       </c>
       <c r="F72" s="3" t="s">
         <v>15</v>
@@ -8178,7 +8191,7 @@
         <v>53</v>
       </c>
       <c r="AA72" s="25" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="AB72" s="3">
         <v>69</v>
@@ -8191,7 +8204,7 @@
     </row>
     <row r="73" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="26" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B73" s="18" t="s">
         <v>33</v>
@@ -8200,11 +8213,11 @@
         <v>0</v>
       </c>
       <c r="D73" s="10">
-        <v>1010111</v>
+        <v>1010110</v>
       </c>
       <c r="E73" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x57</v>
+        <v>0x56</v>
       </c>
       <c r="F73" s="3" t="s">
         <v>15</v>
@@ -8270,7 +8283,7 @@
         <v>53</v>
       </c>
       <c r="AA73" s="25" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AB73" s="3">
         <v>70</v>
@@ -8283,7 +8296,7 @@
     </row>
     <row r="74" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="26" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B74" s="18" t="s">
         <v>33</v>
@@ -8292,11 +8305,11 @@
         <v>0</v>
       </c>
       <c r="D74" s="10">
-        <v>1011000</v>
+        <v>1010111</v>
       </c>
       <c r="E74" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x58</v>
+        <v>0x57</v>
       </c>
       <c r="F74" s="3" t="s">
         <v>15</v>
@@ -8362,7 +8375,7 @@
         <v>53</v>
       </c>
       <c r="AA74" s="25" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AB74" s="3">
         <v>71</v>
@@ -8375,7 +8388,7 @@
     </row>
     <row r="75" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="26" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B75" s="18" t="s">
         <v>33</v>
@@ -8384,11 +8397,11 @@
         <v>0</v>
       </c>
       <c r="D75" s="10">
-        <v>1011001</v>
+        <v>1011000</v>
       </c>
       <c r="E75" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x59</v>
+        <v>0x58</v>
       </c>
       <c r="F75" s="3" t="s">
         <v>15</v>
@@ -8454,7 +8467,7 @@
         <v>53</v>
       </c>
       <c r="AA75" s="25" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="AB75" s="3">
         <v>72</v>
@@ -8467,7 +8480,7 @@
     </row>
     <row r="76" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="26" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B76" s="18" t="s">
         <v>33</v>
@@ -8476,11 +8489,11 @@
         <v>0</v>
       </c>
       <c r="D76" s="10">
-        <v>1011010</v>
+        <v>1011001</v>
       </c>
       <c r="E76" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x5A</v>
+        <v>0x59</v>
       </c>
       <c r="F76" s="3" t="s">
         <v>15</v>
@@ -8546,7 +8559,7 @@
         <v>53</v>
       </c>
       <c r="AA76" s="25" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AB76" s="3">
         <v>73</v>
@@ -8559,7 +8572,7 @@
     </row>
     <row r="77" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="26" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B77" s="18" t="s">
         <v>33</v>
@@ -8568,11 +8581,11 @@
         <v>0</v>
       </c>
       <c r="D77" s="10">
-        <v>1011011</v>
+        <v>1011010</v>
       </c>
       <c r="E77" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x5B</v>
+        <v>0x5A</v>
       </c>
       <c r="F77" s="3" t="s">
         <v>15</v>
@@ -8638,7 +8651,7 @@
         <v>53</v>
       </c>
       <c r="AA77" s="25" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AB77" s="3">
         <v>74</v>
@@ -8651,7 +8664,7 @@
     </row>
     <row r="78" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="26" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B78" s="18" t="s">
         <v>33</v>
@@ -8660,11 +8673,11 @@
         <v>0</v>
       </c>
       <c r="D78" s="10">
-        <v>1011100</v>
+        <v>1011011</v>
       </c>
       <c r="E78" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x5C</v>
+        <v>0x5B</v>
       </c>
       <c r="F78" s="3" t="s">
         <v>15</v>
@@ -8730,7 +8743,7 @@
         <v>53</v>
       </c>
       <c r="AA78" s="25" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AB78" s="3">
         <v>75</v>
@@ -8743,7 +8756,7 @@
     </row>
     <row r="79" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="26" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B79" s="18" t="s">
         <v>33</v>
@@ -8752,11 +8765,11 @@
         <v>0</v>
       </c>
       <c r="D79" s="10">
-        <v>1011101</v>
+        <v>1011100</v>
       </c>
       <c r="E79" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x5D</v>
+        <v>0x5C</v>
       </c>
       <c r="F79" s="3" t="s">
         <v>15</v>
@@ -8822,7 +8835,7 @@
         <v>53</v>
       </c>
       <c r="AA79" s="25" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="AB79" s="3">
         <v>76</v>
@@ -8835,7 +8848,7 @@
     </row>
     <row r="80" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="26" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B80" s="18" t="s">
         <v>33</v>
@@ -8844,11 +8857,11 @@
         <v>0</v>
       </c>
       <c r="D80" s="10">
-        <v>1011110</v>
+        <v>1011101</v>
       </c>
       <c r="E80" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x5E</v>
+        <v>0x5D</v>
       </c>
       <c r="F80" s="3" t="s">
         <v>15</v>
@@ -8914,7 +8927,7 @@
         <v>53</v>
       </c>
       <c r="AA80" s="25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AB80" s="3">
         <v>77</v>
@@ -8927,7 +8940,7 @@
     </row>
     <row r="81" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="26" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B81" s="18" t="s">
         <v>33</v>
@@ -8936,11 +8949,11 @@
         <v>0</v>
       </c>
       <c r="D81" s="10">
-        <v>1011111</v>
+        <v>1011110</v>
       </c>
       <c r="E81" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x5F</v>
+        <v>0x5E</v>
       </c>
       <c r="F81" s="3" t="s">
         <v>15</v>
@@ -9006,7 +9019,7 @@
         <v>53</v>
       </c>
       <c r="AA81" s="25" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AB81" s="3">
         <v>78</v>
@@ -9019,7 +9032,7 @@
     </row>
     <row r="82" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B82" s="18" t="s">
         <v>33</v>
@@ -9028,11 +9041,11 @@
         <v>0</v>
       </c>
       <c r="D82" s="10">
-        <v>1100000</v>
+        <v>1011111</v>
       </c>
       <c r="E82" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x60</v>
+        <v>0x5F</v>
       </c>
       <c r="F82" s="3" t="s">
         <v>15</v>
@@ -9098,7 +9111,7 @@
         <v>53</v>
       </c>
       <c r="AA82" s="25" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AB82" s="3">
         <v>79</v>
@@ -9111,7 +9124,7 @@
     </row>
     <row r="83" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="26" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B83" s="18" t="s">
         <v>33</v>
@@ -9120,11 +9133,11 @@
         <v>0</v>
       </c>
       <c r="D83" s="10">
-        <v>1100001</v>
+        <v>1100000</v>
       </c>
       <c r="E83" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x61</v>
+        <v>0x60</v>
       </c>
       <c r="F83" s="3" t="s">
         <v>15</v>
@@ -9190,7 +9203,7 @@
         <v>53</v>
       </c>
       <c r="AA83" s="25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="AB83" s="3">
         <v>80</v>
@@ -9203,7 +9216,7 @@
     </row>
     <row r="84" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="26" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B84" s="18" t="s">
         <v>33</v>
@@ -9212,11 +9225,11 @@
         <v>0</v>
       </c>
       <c r="D84" s="10">
-        <v>1100010</v>
+        <v>1100001</v>
       </c>
       <c r="E84" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x62</v>
+        <v>0x61</v>
       </c>
       <c r="F84" s="3" t="s">
         <v>15</v>
@@ -9282,7 +9295,7 @@
         <v>53</v>
       </c>
       <c r="AA84" s="25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AB84" s="3">
         <v>81</v>
@@ -9295,7 +9308,7 @@
     </row>
     <row r="85" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="26" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B85" s="18" t="s">
         <v>33</v>
@@ -9304,11 +9317,11 @@
         <v>0</v>
       </c>
       <c r="D85" s="10">
-        <v>1100011</v>
+        <v>1100010</v>
       </c>
       <c r="E85" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x63</v>
+        <v>0x62</v>
       </c>
       <c r="F85" s="3" t="s">
         <v>15</v>
@@ -9374,7 +9387,7 @@
         <v>53</v>
       </c>
       <c r="AA85" s="25" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AB85" s="3">
         <v>82</v>
@@ -9387,7 +9400,7 @@
     </row>
     <row r="86" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="26" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B86" s="18" t="s">
         <v>33</v>
@@ -9396,11 +9409,11 @@
         <v>0</v>
       </c>
       <c r="D86" s="10">
-        <v>1100100</v>
+        <v>1100011</v>
       </c>
       <c r="E86" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x64</v>
+        <v>0x63</v>
       </c>
       <c r="F86" s="3" t="s">
         <v>15</v>
@@ -9466,7 +9479,7 @@
         <v>53</v>
       </c>
       <c r="AA86" s="25" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AB86" s="3">
         <v>83</v>
@@ -9479,7 +9492,7 @@
     </row>
     <row r="87" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="26" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B87" s="18" t="s">
         <v>33</v>
@@ -9488,11 +9501,11 @@
         <v>0</v>
       </c>
       <c r="D87" s="10">
-        <v>1100101</v>
+        <v>1100100</v>
       </c>
       <c r="E87" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x65</v>
+        <v>0x64</v>
       </c>
       <c r="F87" s="3" t="s">
         <v>15</v>
@@ -9558,7 +9571,7 @@
         <v>53</v>
       </c>
       <c r="AA87" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="AB87" s="3">
         <v>84</v>
@@ -9571,7 +9584,7 @@
     </row>
     <row r="88" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="26" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B88" s="18" t="s">
         <v>33</v>
@@ -9580,11 +9593,11 @@
         <v>0</v>
       </c>
       <c r="D88" s="10">
-        <v>1100110</v>
+        <v>1100101</v>
       </c>
       <c r="E88" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x66</v>
+        <v>0x65</v>
       </c>
       <c r="F88" s="3" t="s">
         <v>15</v>
@@ -9650,7 +9663,7 @@
         <v>53</v>
       </c>
       <c r="AA88" s="25" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AB88" s="3">
         <v>85</v>
@@ -9663,7 +9676,7 @@
     </row>
     <row r="89" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="26" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B89" s="18" t="s">
         <v>33</v>
@@ -9672,11 +9685,11 @@
         <v>0</v>
       </c>
       <c r="D89" s="10">
-        <v>1100111</v>
+        <v>1100110</v>
       </c>
       <c r="E89" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x67</v>
+        <v>0x66</v>
       </c>
       <c r="F89" s="3" t="s">
         <v>15</v>
@@ -9742,7 +9755,7 @@
         <v>53</v>
       </c>
       <c r="AA89" s="25" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AB89" s="3">
         <v>86</v>
@@ -9755,7 +9768,7 @@
     </row>
     <row r="90" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B90" s="18" t="s">
         <v>33</v>
@@ -9764,11 +9777,11 @@
         <v>0</v>
       </c>
       <c r="D90" s="10">
-        <v>1101000</v>
+        <v>1100111</v>
       </c>
       <c r="E90" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x68</v>
+        <v>0x67</v>
       </c>
       <c r="F90" s="3" t="s">
         <v>15</v>
@@ -9834,7 +9847,7 @@
         <v>53</v>
       </c>
       <c r="AA90" s="25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AB90" s="3">
         <v>87</v>
@@ -9847,7 +9860,7 @@
     </row>
     <row r="91" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="26" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B91" s="18" t="s">
         <v>33</v>
@@ -9856,11 +9869,11 @@
         <v>0</v>
       </c>
       <c r="D91" s="10">
-        <v>1101001</v>
+        <v>1101000</v>
       </c>
       <c r="E91" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x69</v>
+        <v>0x68</v>
       </c>
       <c r="F91" s="3" t="s">
         <v>15</v>
@@ -9926,7 +9939,7 @@
         <v>53</v>
       </c>
       <c r="AA91" s="25" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AB91" s="3">
         <v>88</v>
@@ -9939,7 +9952,7 @@
     </row>
     <row r="92" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B92" s="18" t="s">
         <v>33</v>
@@ -9948,11 +9961,11 @@
         <v>0</v>
       </c>
       <c r="D92" s="10">
-        <v>1101010</v>
+        <v>1101001</v>
       </c>
       <c r="E92" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x6A</v>
+        <v>0x69</v>
       </c>
       <c r="F92" s="3" t="s">
         <v>15</v>
@@ -10018,7 +10031,7 @@
         <v>53</v>
       </c>
       <c r="AA92" s="25" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AB92" s="3">
         <v>89</v>
@@ -10031,7 +10044,7 @@
     </row>
     <row r="93" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B93" s="18" t="s">
         <v>33</v>
@@ -10040,11 +10053,11 @@
         <v>0</v>
       </c>
       <c r="D93" s="10">
-        <v>1101011</v>
+        <v>1101010</v>
       </c>
       <c r="E93" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x6B</v>
+        <v>0x6A</v>
       </c>
       <c r="F93" s="3" t="s">
         <v>15</v>
@@ -10110,7 +10123,7 @@
         <v>53</v>
       </c>
       <c r="AA93" s="25" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AB93" s="3">
         <v>90</v>
@@ -10123,7 +10136,7 @@
     </row>
     <row r="94" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="26" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B94" s="18" t="s">
         <v>33</v>
@@ -10132,11 +10145,11 @@
         <v>0</v>
       </c>
       <c r="D94" s="10">
-        <v>1101100</v>
+        <v>1101011</v>
       </c>
       <c r="E94" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x6C</v>
+        <v>0x6B</v>
       </c>
       <c r="F94" s="3" t="s">
         <v>15</v>
@@ -10202,7 +10215,7 @@
         <v>53</v>
       </c>
       <c r="AA94" s="25" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AB94" s="3">
         <v>91</v>
@@ -10215,7 +10228,7 @@
     </row>
     <row r="95" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="26" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B95" s="18" t="s">
         <v>33</v>
@@ -10224,11 +10237,11 @@
         <v>0</v>
       </c>
       <c r="D95" s="10">
-        <v>1101101</v>
+        <v>1101100</v>
       </c>
       <c r="E95" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x6D</v>
+        <v>0x6C</v>
       </c>
       <c r="F95" s="3" t="s">
         <v>15</v>
@@ -10294,7 +10307,7 @@
         <v>53</v>
       </c>
       <c r="AA95" s="25" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AB95" s="3">
         <v>92</v>
@@ -10307,7 +10320,7 @@
     </row>
     <row r="96" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="26" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B96" s="18" t="s">
         <v>33</v>
@@ -10316,11 +10329,11 @@
         <v>0</v>
       </c>
       <c r="D96" s="10">
-        <v>1101110</v>
+        <v>1101101</v>
       </c>
       <c r="E96" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x6E</v>
+        <v>0x6D</v>
       </c>
       <c r="F96" s="3" t="s">
         <v>15</v>
@@ -10386,7 +10399,7 @@
         <v>53</v>
       </c>
       <c r="AA96" s="25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AB96" s="3">
         <v>93</v>
@@ -10399,7 +10412,7 @@
     </row>
     <row r="97" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="26" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B97" s="18" t="s">
         <v>33</v>
@@ -10408,11 +10421,11 @@
         <v>0</v>
       </c>
       <c r="D97" s="10">
-        <v>1101111</v>
+        <v>1101110</v>
       </c>
       <c r="E97" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x6F</v>
+        <v>0x6E</v>
       </c>
       <c r="F97" s="3" t="s">
         <v>15</v>
@@ -10478,7 +10491,7 @@
         <v>53</v>
       </c>
       <c r="AA97" s="25" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AB97" s="3">
         <v>94</v>
@@ -10491,7 +10504,7 @@
     </row>
     <row r="98" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="26" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B98" s="18" t="s">
         <v>33</v>
@@ -10500,11 +10513,11 @@
         <v>0</v>
       </c>
       <c r="D98" s="10">
-        <v>1110000</v>
+        <v>1101111</v>
       </c>
       <c r="E98" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x70</v>
+        <v>0x6F</v>
       </c>
       <c r="F98" s="3" t="s">
         <v>15</v>
@@ -10570,7 +10583,7 @@
         <v>53</v>
       </c>
       <c r="AA98" s="25" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AB98" s="3">
         <v>95</v>
@@ -10583,7 +10596,7 @@
     </row>
     <row r="99" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B99" s="18" t="s">
         <v>33</v>
@@ -10592,11 +10605,11 @@
         <v>0</v>
       </c>
       <c r="D99" s="10">
-        <v>1110001</v>
+        <v>1110000</v>
       </c>
       <c r="E99" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x71</v>
+        <v>0x70</v>
       </c>
       <c r="F99" s="3" t="s">
         <v>15</v>
@@ -10662,7 +10675,7 @@
         <v>53</v>
       </c>
       <c r="AA99" s="25" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="AB99" s="3">
         <v>96</v>
@@ -10675,7 +10688,7 @@
     </row>
     <row r="100" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="26" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B100" s="18" t="s">
         <v>33</v>
@@ -10684,11 +10697,11 @@
         <v>0</v>
       </c>
       <c r="D100" s="10">
-        <v>1110010</v>
+        <v>1110001</v>
       </c>
       <c r="E100" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x72</v>
+        <v>0x71</v>
       </c>
       <c r="F100" s="3" t="s">
         <v>15</v>
@@ -10754,7 +10767,7 @@
         <v>53</v>
       </c>
       <c r="AA100" s="25" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AB100" s="3">
         <v>97</v>
@@ -10767,7 +10780,7 @@
     </row>
     <row r="101" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B101" s="18" t="s">
         <v>33</v>
@@ -10776,11 +10789,11 @@
         <v>0</v>
       </c>
       <c r="D101" s="10">
-        <v>1110011</v>
+        <v>1110010</v>
       </c>
       <c r="E101" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x73</v>
+        <v>0x72</v>
       </c>
       <c r="F101" s="3" t="s">
         <v>15</v>
@@ -10846,7 +10859,7 @@
         <v>53</v>
       </c>
       <c r="AA101" s="25" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AB101" s="3">
         <v>98</v>
@@ -10859,7 +10872,7 @@
     </row>
     <row r="102" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="26" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B102" s="18" t="s">
         <v>33</v>
@@ -10868,11 +10881,11 @@
         <v>0</v>
       </c>
       <c r="D102" s="10">
-        <v>1110100</v>
+        <v>1110011</v>
       </c>
       <c r="E102" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x74</v>
+        <v>0x73</v>
       </c>
       <c r="F102" s="3" t="s">
         <v>15</v>
@@ -10938,7 +10951,7 @@
         <v>53</v>
       </c>
       <c r="AA102" s="25" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AB102" s="3">
         <v>99</v>
@@ -10951,7 +10964,7 @@
     </row>
     <row r="103" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="26" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B103" s="18" t="s">
         <v>33</v>
@@ -10960,11 +10973,11 @@
         <v>0</v>
       </c>
       <c r="D103" s="10">
-        <v>1110101</v>
+        <v>1110100</v>
       </c>
       <c r="E103" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x75</v>
+        <v>0x74</v>
       </c>
       <c r="F103" s="3" t="s">
         <v>15</v>
@@ -11030,7 +11043,7 @@
         <v>53</v>
       </c>
       <c r="AA103" s="25" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AB103" s="3">
         <v>100</v>
@@ -11043,7 +11056,7 @@
     </row>
     <row r="104" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="26" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B104" s="18" t="s">
         <v>33</v>
@@ -11052,11 +11065,11 @@
         <v>0</v>
       </c>
       <c r="D104" s="10">
-        <v>1110110</v>
+        <v>1110101</v>
       </c>
       <c r="E104" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x76</v>
+        <v>0x75</v>
       </c>
       <c r="F104" s="3" t="s">
         <v>15</v>
@@ -11122,7 +11135,7 @@
         <v>53</v>
       </c>
       <c r="AA104" s="25" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AB104" s="3">
         <v>101</v>
@@ -11135,7 +11148,7 @@
     </row>
     <row r="105" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="26" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B105" s="18" t="s">
         <v>33</v>
@@ -11144,11 +11157,11 @@
         <v>0</v>
       </c>
       <c r="D105" s="10">
-        <v>1110111</v>
+        <v>1110110</v>
       </c>
       <c r="E105" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x77</v>
+        <v>0x76</v>
       </c>
       <c r="F105" s="3" t="s">
         <v>15</v>
@@ -11214,7 +11227,7 @@
         <v>53</v>
       </c>
       <c r="AA105" s="25" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AB105" s="3">
         <v>102</v>
@@ -11227,7 +11240,7 @@
     </row>
     <row r="106" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B106" s="18" t="s">
         <v>33</v>
@@ -11236,11 +11249,11 @@
         <v>0</v>
       </c>
       <c r="D106" s="10">
-        <v>1111000</v>
+        <v>1110111</v>
       </c>
       <c r="E106" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x78</v>
+        <v>0x77</v>
       </c>
       <c r="F106" s="3" t="s">
         <v>15</v>
@@ -11306,7 +11319,7 @@
         <v>53</v>
       </c>
       <c r="AA106" s="25" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AB106" s="3">
         <v>103</v>
@@ -11319,7 +11332,7 @@
     </row>
     <row r="107" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="26" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B107" s="18" t="s">
         <v>33</v>
@@ -11328,11 +11341,11 @@
         <v>0</v>
       </c>
       <c r="D107" s="10">
-        <v>1111001</v>
+        <v>1111000</v>
       </c>
       <c r="E107" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x79</v>
+        <v>0x78</v>
       </c>
       <c r="F107" s="3" t="s">
         <v>15</v>
@@ -11398,7 +11411,7 @@
         <v>53</v>
       </c>
       <c r="AA107" s="25" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AB107" s="3">
         <v>104</v>
@@ -11411,7 +11424,7 @@
     </row>
     <row r="108" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B108" s="18" t="s">
         <v>33</v>
@@ -11420,11 +11433,11 @@
         <v>0</v>
       </c>
       <c r="D108" s="10">
-        <v>1111010</v>
+        <v>1111001</v>
       </c>
       <c r="E108" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x7A</v>
+        <v>0x79</v>
       </c>
       <c r="F108" s="3" t="s">
         <v>15</v>
@@ -11490,7 +11503,7 @@
         <v>53</v>
       </c>
       <c r="AA108" s="25" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AB108" s="3">
         <v>105</v>
@@ -11503,7 +11516,7 @@
     </row>
     <row r="109" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="26" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B109" s="18" t="s">
         <v>33</v>
@@ -11512,11 +11525,11 @@
         <v>0</v>
       </c>
       <c r="D109" s="10">
-        <v>1111011</v>
+        <v>1111010</v>
       </c>
       <c r="E109" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x7B</v>
+        <v>0x7A</v>
       </c>
       <c r="F109" s="3" t="s">
         <v>15</v>
@@ -11582,7 +11595,7 @@
         <v>53</v>
       </c>
       <c r="AA109" s="25" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AB109" s="3">
         <v>106</v>
@@ -11595,7 +11608,7 @@
     </row>
     <row r="110" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="26" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B110" s="18" t="s">
         <v>33</v>
@@ -11604,11 +11617,11 @@
         <v>0</v>
       </c>
       <c r="D110" s="10">
-        <v>1111100</v>
+        <v>1111011</v>
       </c>
       <c r="E110" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x7C</v>
+        <v>0x7B</v>
       </c>
       <c r="F110" s="3" t="s">
         <v>15</v>
@@ -11674,7 +11687,7 @@
         <v>53</v>
       </c>
       <c r="AA110" s="25" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AB110" s="3">
         <v>107</v>
@@ -11687,7 +11700,7 @@
     </row>
     <row r="111" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="26" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B111" s="18" t="s">
         <v>33</v>
@@ -11696,11 +11709,11 @@
         <v>0</v>
       </c>
       <c r="D111" s="10">
-        <v>1111101</v>
+        <v>1111100</v>
       </c>
       <c r="E111" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x7D</v>
+        <v>0x7C</v>
       </c>
       <c r="F111" s="3" t="s">
         <v>15</v>
@@ -11766,7 +11779,7 @@
         <v>53</v>
       </c>
       <c r="AA111" s="25" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AB111" s="3">
         <v>108</v>
@@ -11779,7 +11792,7 @@
     </row>
     <row r="112" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="26" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B112" s="18" t="s">
         <v>33</v>
@@ -11788,11 +11801,11 @@
         <v>0</v>
       </c>
       <c r="D112" s="10">
-        <v>1111110</v>
+        <v>1111101</v>
       </c>
       <c r="E112" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x7E</v>
+        <v>0x7D</v>
       </c>
       <c r="F112" s="3" t="s">
         <v>15</v>
@@ -11858,7 +11871,7 @@
         <v>53</v>
       </c>
       <c r="AA112" s="25" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AB112" s="3">
         <v>109</v>
@@ -11871,7 +11884,7 @@
     </row>
     <row r="113" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="26" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B113" s="18" t="s">
         <v>33</v>
@@ -11880,11 +11893,11 @@
         <v>0</v>
       </c>
       <c r="D113" s="10">
-        <v>1111111</v>
+        <v>1111110</v>
       </c>
       <c r="E113" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x7F</v>
+        <v>0x7E</v>
       </c>
       <c r="F113" s="3" t="s">
         <v>15</v>
@@ -11950,7 +11963,7 @@
         <v>53</v>
       </c>
       <c r="AA113" s="25" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AB113" s="3">
         <v>110</v>
@@ -11963,7 +11976,7 @@
     </row>
     <row r="114" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="26" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B114" s="18" t="s">
         <v>33</v>
@@ -11972,11 +11985,11 @@
         <v>0</v>
       </c>
       <c r="D114" s="10">
-        <v>1</v>
+        <v>1111111</v>
       </c>
       <c r="E114" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x1</v>
+        <v>0x7F</v>
       </c>
       <c r="F114" s="3" t="s">
         <v>15</v>
@@ -12042,7 +12055,7 @@
         <v>53</v>
       </c>
       <c r="AA114" s="25" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AB114" s="3">
         <v>111</v>
@@ -12054,8 +12067,8 @@
       <c r="AE114" s="3"/>
     </row>
     <row r="115" spans="1:31" ht="16" x14ac:dyDescent="0.2">
-      <c r="A115" s="3" t="s">
-        <v>52</v>
+      <c r="A115" s="26" t="s">
+        <v>244</v>
       </c>
       <c r="B115" s="18" t="s">
         <v>33</v>
@@ -12064,11 +12077,11 @@
         <v>0</v>
       </c>
       <c r="D115" s="10">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="E115" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x4</v>
+        <v>0x1</v>
       </c>
       <c r="F115" s="3" t="s">
         <v>15</v>
@@ -12133,8 +12146,8 @@
       <c r="Z115" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AA115" s="23" t="s">
-        <v>71</v>
+      <c r="AA115" s="25" t="s">
+        <v>312</v>
       </c>
       <c r="AB115" s="3">
         <v>112</v>
@@ -12142,26 +12155,118 @@
       <c r="AC115" s="26" t="s">
         <v>316</v>
       </c>
-      <c r="AD115" t="s">
+      <c r="AD115" s="3"/>
+      <c r="AE115" s="3"/>
+    </row>
+    <row r="116" spans="1:31" ht="16" x14ac:dyDescent="0.2">
+      <c r="A116" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B116" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C116" s="3">
+        <v>0</v>
+      </c>
+      <c r="D116" s="10">
+        <v>100</v>
+      </c>
+      <c r="E116" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0x4</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G116" t="s">
+        <v>15</v>
+      </c>
+      <c r="H116" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I116" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J116" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K116" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="L116" s="6">
+        <v>0</v>
+      </c>
+      <c r="M116" s="6">
+        <v>0</v>
+      </c>
+      <c r="N116" s="6">
+        <v>0</v>
+      </c>
+      <c r="O116" s="6">
+        <v>0</v>
+      </c>
+      <c r="P116" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q116" s="6">
+        <v>0</v>
+      </c>
+      <c r="R116" s="6">
+        <v>0</v>
+      </c>
+      <c r="S116" s="6">
+        <v>0</v>
+      </c>
+      <c r="T116" s="6">
+        <v>1</v>
+      </c>
+      <c r="U116" s="6">
+        <v>0</v>
+      </c>
+      <c r="V116" s="6">
+        <v>0</v>
+      </c>
+      <c r="W116" s="16">
+        <v>0</v>
+      </c>
+      <c r="X116" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y116" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z116" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA116" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB116" s="3">
+        <v>113</v>
+      </c>
+      <c r="AC116" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="AD116" t="s">
         <v>35</v>
       </c>
-      <c r="AE115" t="s">
+      <c r="AE116" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="116" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="L116" s="6"/>
-      <c r="M116" s="6"/>
-      <c r="N116" s="6"/>
-      <c r="O116" s="6"/>
-      <c r="P116" s="6"/>
-      <c r="Q116" s="6"/>
-      <c r="R116" s="6"/>
-      <c r="S116" s="6"/>
-      <c r="T116" s="6"/>
-      <c r="U116" s="6"/>
-      <c r="V116" s="6"/>
-      <c r="W116" s="16"/>
+    <row r="117" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="L117" s="6"/>
+      <c r="M117" s="6"/>
+      <c r="N117" s="6"/>
+      <c r="O117" s="6"/>
+      <c r="P117" s="6"/>
+      <c r="Q117" s="6"/>
+      <c r="R117" s="6"/>
+      <c r="S117" s="6"/>
+      <c r="T117" s="6"/>
+      <c r="U117" s="6"/>
+      <c r="V117" s="6"/>
+      <c r="W117" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>